<commit_message>
modified details reports formula
</commit_message>
<xml_diff>
--- a/WatanyaPingTester/bin/Debug/res/alexColorReport.xlsx
+++ b/WatanyaPingTester/bin/Debug/res/alexColorReport.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fahim\Pingo\WatanyaPingTester\bin\Debug\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Fahim\C#\New folder\Pingo\WatanyaPingTester\bin\Debug\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="9900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2895" windowHeight="720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,8 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="89">
   <si>
-    <t>From: 0716 To: 0746</t>
+    <t>From: 23/01/2018 at 1232
+To: 23/01/2018 at 1247</t>
   </si>
   <si>
     <t>El Sheikh Zaid Gate:</t>
@@ -357,13 +358,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,7 +658,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -664,1245 +668,1249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B5" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C5" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D5" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E5" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F5" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B6" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D6" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E6" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F6" s="6">
+        <v>99.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F11" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B11" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C11" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D11" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E11" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F11" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B12" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D12" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E12" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="F12" s="6">
+        <v>99.83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B17" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C17" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D17" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E17" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F17" s="5">
-        <v>85.41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B18" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C18" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D18" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E18" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F18" s="6">
+        <v>82.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F23" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B23" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C23" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D23" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E23" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F23" s="5">
-        <v>85.41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B24" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C24" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D24" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E24" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F24" s="6">
+        <v>82.36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F26" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F27" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="B27" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="C27" s="5">
-        <v>98.54</v>
-      </c>
-      <c r="D27" s="5">
-        <v>73.13</v>
-      </c>
-      <c r="E27" s="5">
-        <v>66.52</v>
-      </c>
-      <c r="F27" s="5">
-        <v>65.319999999999993</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A30" s="4" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>99</v>
+      </c>
+      <c r="B28" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="C28" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="D28" s="6">
+        <v>77.37</v>
+      </c>
+      <c r="E28" s="6">
+        <v>73.88</v>
+      </c>
+      <c r="F28" s="6">
+        <v>71.55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F32" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F33" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B33" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C33" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D33" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E33" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F33" s="5">
-        <v>85.41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B34" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C34" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D34" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E34" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F34" s="6">
+        <v>82.36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>99.06</v>
-      </c>
-      <c r="B37" s="5">
-        <v>99.57</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A40" s="4" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="B38" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A41" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D42" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E42" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F42" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F43" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B43" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C43" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D43" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E43" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F43" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B44" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C44" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D44" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E44" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F44" s="6">
+        <v>97.67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D46" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B47" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C47" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B47" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="C47" s="5">
-        <v>94.42</v>
-      </c>
-      <c r="D47" s="5">
-        <v>25.92</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A50" s="4" t="s">
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>88.02</v>
+      </c>
+      <c r="B48" s="6">
+        <v>0</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+      <c r="D48" s="6">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A51" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D52" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E52" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F52" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C53" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D53" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E53" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F53" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B53" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C53" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D53" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E53" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F53" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B54" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C54" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D54" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E54" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F54" s="6">
+        <v>99.33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D56" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B57" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C57" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D57" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
-        <v>99.14</v>
-      </c>
-      <c r="B57" s="5">
-        <v>99.66</v>
-      </c>
-      <c r="C57" s="5">
-        <v>99.31</v>
-      </c>
-      <c r="D57" s="5">
-        <v>99.4</v>
-      </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A60" s="4" t="s">
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>94.51</v>
+      </c>
+      <c r="B58" s="6">
+        <v>94.84</v>
+      </c>
+      <c r="C58" s="6">
+        <v>95.51</v>
+      </c>
+      <c r="D58" s="6">
+        <v>95.01</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A61" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="4"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B62" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C62" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D62" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E62" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F62" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B63" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C63" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D63" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E63" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F63" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B63" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C63" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D63" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E63" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F63" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B64" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C64" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D64" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E64" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F64" s="6">
+        <v>99.33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B66" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C66" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D66" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B67" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C67" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D67" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
-        <v>99.14</v>
-      </c>
-      <c r="B67" s="5">
-        <v>99.66</v>
-      </c>
-      <c r="C67" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="D67" s="5">
-        <v>99.48</v>
-      </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A70" s="4" t="s">
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>94.51</v>
+      </c>
+      <c r="B68" s="6">
+        <v>94.84</v>
+      </c>
+      <c r="C68" s="6">
+        <v>92.68</v>
+      </c>
+      <c r="D68" s="6">
+        <v>93.01</v>
+      </c>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+    </row>
+    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A71" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="4"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B72" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C72" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D72" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E72" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F72" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B73" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C73" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D73" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E73" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F73" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B73" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C73" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D73" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E73" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F73" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B74" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C74" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D74" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E74" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F74" s="6">
+        <v>99.33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B76" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C76" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D76" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E76" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F76" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B77" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C77" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D77" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E77" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F77" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <v>99.14</v>
-      </c>
-      <c r="B77" s="5">
-        <v>99.66</v>
-      </c>
-      <c r="C77" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D77" s="5">
-        <v>99.31</v>
-      </c>
-      <c r="E77" s="5">
-        <v>99.57</v>
-      </c>
-      <c r="F77" s="5">
-        <v>99.31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A80" s="4" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>94.51</v>
+      </c>
+      <c r="B78" s="6">
+        <v>94.84</v>
+      </c>
+      <c r="C78" s="6">
+        <v>92.85</v>
+      </c>
+      <c r="D78" s="6">
+        <v>94.34</v>
+      </c>
+      <c r="E78" s="6">
+        <v>93.51</v>
+      </c>
+      <c r="F78" s="6">
+        <v>94.68</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A81" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B80" s="4"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B82" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C82" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D82" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="E82" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F82" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B83" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C83" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D83" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E83" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="F83" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B83" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C83" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D83" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E83" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F83" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B84" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C84" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D84" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E84" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F84" s="6">
+        <v>99.33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B86" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B87" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B87" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A90" s="4" t="s">
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>94.34</v>
+      </c>
+      <c r="B88" s="6">
+        <v>95.84</v>
+      </c>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+    </row>
+    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A91" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B90" s="4"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+      <c r="B91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B92" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C92" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D92" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E92" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F92" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B93" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C93" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D93" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E93" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F93" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="B93" s="5">
-        <v>99.74</v>
-      </c>
-      <c r="C93" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D93" s="5">
-        <v>99.23</v>
-      </c>
-      <c r="E93" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="F93" s="5">
-        <v>99.91</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="B94" s="6">
+        <v>99.5</v>
+      </c>
+      <c r="C94" s="6">
+        <v>99.33</v>
+      </c>
+      <c r="D94" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="E94" s="6">
+        <v>99.83</v>
+      </c>
+      <c r="F94" s="6">
+        <v>99.33</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B96" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C96" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D96" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E96" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F96" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B97" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C97" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D97" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E96" s="5" t="s">
+      <c r="E97" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F96" s="5" t="s">
+      <c r="F97" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
-        <v>99.14</v>
-      </c>
-      <c r="B97" s="5">
-        <v>99.66</v>
-      </c>
-      <c r="C97" s="5">
-        <v>99.91</v>
-      </c>
-      <c r="D97" s="5">
-        <v>99.31</v>
-      </c>
-      <c r="E97" s="5">
-        <v>90.9</v>
-      </c>
-      <c r="F97" s="5">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>94.51</v>
+      </c>
+      <c r="B98" s="6">
+        <v>94.84</v>
+      </c>
+      <c r="C98" s="6">
+        <v>92.85</v>
+      </c>
+      <c r="D98" s="6">
+        <v>94.34</v>
+      </c>
+      <c r="E98" s="6">
+        <v>86.86</v>
+      </c>
+      <c r="F98" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B100" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C100" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D100" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E99" s="5" t="s">
+      <c r="E100" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="F100" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B101" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C101" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D101" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E101" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="F101" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="5">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="6">
         <v>0</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B102" s="6">
         <v>0</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="6">
         <v>0</v>
       </c>
-      <c r="D101" s="5">
+      <c r="D102" s="6">
         <v>0</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E102" s="6">
         <v>0</v>
       </c>
-      <c r="F101" s="5">
+      <c r="F102" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B104" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B105" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="5">
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="6">
         <v>0</v>
       </c>
-      <c r="B105" s="5">
+      <c r="B106" s="6">
         <v>0</v>
       </c>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:F5">
+  <conditionalFormatting sqref="A6:F6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1952,7 +1960,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:F11">
+  <conditionalFormatting sqref="A12:F12">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2002,7 +2010,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:F17">
+  <conditionalFormatting sqref="A18:F18">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2052,7 +2060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:F23">
+  <conditionalFormatting sqref="A24:F24">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2102,7 +2110,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:F27">
+  <conditionalFormatting sqref="A28:F28">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2152,7 +2160,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33:F33">
+  <conditionalFormatting sqref="A34:F34">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -2202,7 +2210,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:F37">
+  <conditionalFormatting sqref="A38:F38">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -2220,7 +2228,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:F43">
+  <conditionalFormatting sqref="A44:F44">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -2270,7 +2278,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47:F47">
+  <conditionalFormatting sqref="A48:F48">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -2304,7 +2312,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:F53">
+  <conditionalFormatting sqref="A54:F54">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -2354,7 +2362,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:F57">
+  <conditionalFormatting sqref="A58:F58">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -2388,7 +2396,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:F63">
+  <conditionalFormatting sqref="A64:F64">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -2438,7 +2446,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A67:F67">
+  <conditionalFormatting sqref="A68:F68">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -2472,7 +2480,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A73:F73">
+  <conditionalFormatting sqref="A74:F74">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -2522,7 +2530,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77:F77">
+  <conditionalFormatting sqref="A78:F78">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
@@ -2572,7 +2580,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A83:F83">
+  <conditionalFormatting sqref="A84:F84">
     <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
@@ -2622,7 +2630,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A87:F87">
+  <conditionalFormatting sqref="A88:F88">
     <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
@@ -2640,7 +2648,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A93:F93">
+  <conditionalFormatting sqref="A94:F94">
     <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
@@ -2690,7 +2698,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A97:F97">
+  <conditionalFormatting sqref="A98:F98">
     <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
@@ -2740,7 +2748,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A101:F101">
+  <conditionalFormatting sqref="A102:F102">
     <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
@@ -2790,7 +2798,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A105:F105">
+  <conditionalFormatting sqref="A106:F106">
     <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
@@ -2800,7 +2808,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A105:F105">
+  <conditionalFormatting sqref="A106:F106">
     <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
@@ -2811,6 +2819,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added xml report module
</commit_message>
<xml_diff>
--- a/WatanyaPingTester/bin/Debug/res/alexColorReport.xlsx
+++ b/WatanyaPingTester/bin/Debug/res/alexColorReport.xlsx
@@ -26,8 +26,8 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="89">
   <si>
-    <t>From: 23/01/2018 at 1232
-To: 23/01/2018 at 1247</t>
+    <t>From: 28/01/2018 at 1745
+To: 28/01/2018 at 1840</t>
   </si>
   <si>
     <t>El Sheikh Zaid Gate:</t>
@@ -725,22 +725,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B6" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C6" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D6" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E6" s="6">
-        <v>99.83</v>
+        <v>99.29</v>
       </c>
       <c r="F6" s="6">
-        <v>99.83</v>
+        <v>96.89</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -791,22 +791,22 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B12" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C12" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D12" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E12" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="F12" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -857,22 +857,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B18" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C18" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D18" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E18" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F18" s="6">
-        <v>82.36</v>
+        <v>90.82</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -923,22 +923,22 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B24" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C24" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D24" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E24" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F24" s="6">
-        <v>82.36</v>
+        <v>90.82</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -983,22 +983,22 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <v>99</v>
+        <v>99.4</v>
       </c>
       <c r="B28" s="6">
-        <v>99.33</v>
+        <v>97.87</v>
       </c>
       <c r="C28" s="6">
-        <v>99.83</v>
+        <v>97.49</v>
       </c>
       <c r="D28" s="6">
-        <v>77.37</v>
+        <v>93.45</v>
       </c>
       <c r="E28" s="6">
-        <v>73.88</v>
+        <v>91.97</v>
       </c>
       <c r="F28" s="6">
-        <v>71.55</v>
+        <v>92.79</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -1049,22 +1049,22 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B34" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C34" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D34" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E34" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F34" s="6">
-        <v>82.36</v>
+        <v>90.82</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1093,10 +1093,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <v>99.5</v>
+        <v>95.85</v>
       </c>
       <c r="B38" s="6">
-        <v>99.83</v>
+        <v>99.4</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1151,22 +1151,22 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B44" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C44" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D44" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E44" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F44" s="6">
-        <v>97.67</v>
+        <v>96.45</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
-        <v>88.02</v>
+        <v>88.42</v>
       </c>
       <c r="B48" s="6">
         <v>0</v>
@@ -1265,22 +1265,22 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B54" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C54" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D54" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E54" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F54" s="6">
-        <v>99.33</v>
+        <v>98.85</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,16 +1317,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
-        <v>94.51</v>
+        <v>92.03</v>
       </c>
       <c r="B58" s="6">
-        <v>94.84</v>
+        <v>91.81</v>
       </c>
       <c r="C58" s="6">
-        <v>95.51</v>
+        <v>93.34</v>
       </c>
       <c r="D58" s="6">
-        <v>95.01</v>
+        <v>92.63</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -1379,22 +1379,22 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B64" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C64" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D64" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E64" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F64" s="6">
-        <v>99.33</v>
+        <v>98.85</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1431,16 +1431,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
-        <v>94.51</v>
+        <v>92.03</v>
       </c>
       <c r="B68" s="6">
-        <v>94.84</v>
+        <v>91.81</v>
       </c>
       <c r="C68" s="6">
-        <v>92.68</v>
+        <v>92.08</v>
       </c>
       <c r="D68" s="6">
-        <v>93.01</v>
+        <v>92.57</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -1493,22 +1493,22 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B74" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C74" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D74" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E74" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F74" s="6">
-        <v>99.33</v>
+        <v>98.85</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1553,22 +1553,22 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
-        <v>94.51</v>
+        <v>92.03</v>
       </c>
       <c r="B78" s="6">
-        <v>94.84</v>
+        <v>91.81</v>
       </c>
       <c r="C78" s="6">
-        <v>92.85</v>
+        <v>93.77</v>
       </c>
       <c r="D78" s="6">
-        <v>94.34</v>
+        <v>86.07</v>
       </c>
       <c r="E78" s="6">
-        <v>93.51</v>
+        <v>85.91</v>
       </c>
       <c r="F78" s="6">
-        <v>94.68</v>
+        <v>84.76</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -1619,22 +1619,22 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B84" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C84" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D84" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E84" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F84" s="6">
-        <v>99.33</v>
+        <v>98.85</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -1663,10 +1663,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
-        <v>94.34</v>
+        <v>92.19</v>
       </c>
       <c r="B88" s="6">
-        <v>95.84</v>
+        <v>90.01</v>
       </c>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
@@ -1721,22 +1721,22 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
-        <v>99.83</v>
+        <v>99.67</v>
       </c>
       <c r="B94" s="6">
-        <v>99.5</v>
+        <v>99.13</v>
       </c>
       <c r="C94" s="6">
-        <v>99.33</v>
+        <v>99.56</v>
       </c>
       <c r="D94" s="6">
-        <v>99.83</v>
+        <v>99.34</v>
       </c>
       <c r="E94" s="6">
-        <v>99.83</v>
+        <v>99.56</v>
       </c>
       <c r="F94" s="6">
-        <v>99.33</v>
+        <v>98.85</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -1781,19 +1781,19 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
-        <v>94.51</v>
+        <v>92.03</v>
       </c>
       <c r="B98" s="6">
-        <v>94.84</v>
+        <v>91.81</v>
       </c>
       <c r="C98" s="6">
-        <v>92.85</v>
+        <v>93.77</v>
       </c>
       <c r="D98" s="6">
-        <v>94.34</v>
+        <v>86.07</v>
       </c>
       <c r="E98" s="6">
-        <v>86.86</v>
+        <v>79.63</v>
       </c>
       <c r="F98" s="6">
         <v>0</v>

</xml_diff>